<commit_message>
Upgraded Utilities and Initial F82H Database
incorporated team's suggestions
</commit_message>
<xml_diff>
--- a/Jupyter/F82H/Eurofer_example_Qihan.xlsx
+++ b/Jupyter/F82H/Eurofer_example_Qihan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Computer Codes\Jupyter\F82H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuqih\Documents\GitHub\DatabaseCodes_QF\Computer Codes\Jupyter\Eurofer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B30F23E-BC3F-4F95-918F-4B04964FA783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A41598-8CF6-4F28-8100-11BE071F6E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19020" yWindow="0" windowWidth="19380" windowHeight="20880" tabRatio="852" firstSheet="2" activeTab="7" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="852" activeTab="8" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Eurofer_diffusivity" sheetId="1" r:id="rId1"/>
@@ -2235,13 +2235,13 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="12.54296875" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="10"/>
+    <col min="1" max="26" width="12.5703125" style="10" customWidth="1"/>
+    <col min="27" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2249,13 +2249,13 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="45.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>295.59585492227899</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>8.1640711902113403E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>322.79792746113901</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>8.0789766407119004E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>373.31606217616502</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>7.7536151279199106E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>472.79792746113901</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>7.5784204671857605E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>573.05699481865202</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>7.0728587319243599E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>673.31606217616502</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>6.4822024471635098E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>772.79792746114003</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>5.8014460511679598E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>873.05699481865202</v>
       </c>
@@ -2328,13 +2328,13 @@
         <v>5.0255839822024397E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="15"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>5</v>
       </c>
@@ -2362,26 +2362,26 @@
       <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="2"/>
-    <col min="4" max="4" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="2"/>
-    <col min="7" max="7" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="2"/>
-    <col min="10" max="10" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="2"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>47</v>
       </c>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="N1" s="15"/>
     </row>
-    <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>10</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>95.557891687808393</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>30</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>88.682804290936701</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>100</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>81.200483429553103</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>300</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>74.529005773187606</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1000</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>66.640813839669093</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>3000</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>60.172496454184</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>10000</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>52.487914261171703</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>30000</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>45.612377394674198</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>100000</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>37.927795201662001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>300000</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>30.849547533909899</v>
       </c>
     </row>
-    <row r="32" spans="13:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
@@ -2768,7 +2768,7 @@
       <c r="V32" s="15"/>
       <c r="W32" s="15"/>
     </row>
-    <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>52</v>
       </c>
@@ -2820,25 +2820,25 @@
       <selection activeCell="P52" sqref="P52:T52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="2" customWidth="1"/>
-    <col min="4" max="5" width="13.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="2"/>
-    <col min="7" max="8" width="13.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="2"/>
-    <col min="10" max="11" width="14.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="2"/>
-    <col min="13" max="14" width="14.7265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.1796875" style="2"/>
-    <col min="16" max="17" width="15.26953125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="9.1796875" style="2"/>
-    <col min="19" max="20" width="15.26953125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="2" width="13.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="13.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="8" width="13.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="10" max="11" width="14.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="2"/>
+    <col min="13" max="14" width="14.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="2"/>
+    <col min="16" max="17" width="15.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="2"/>
+    <col min="19" max="20" width="15.28515625" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>41</v>
       </c>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="T1" s="15"/>
     </row>
-    <row r="3" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4.8638199999999996</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>1.81249999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>9.9451300000000007</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>1.61029411764705</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>24.994789999999998</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>48.371310000000001</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>1.4117647058823499</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>100.27548</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>1.41911764705882</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>252.01924</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>1.41911764705882</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>494.47662000000003</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>1.4117647058823499</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>50270.617209999997</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>1.40808823529411</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>98633.9179</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>1.2242647058823499</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>207303.64079999999</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>1.01838235294117</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>506872.17005999997</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>0.91911764705882304</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1000000</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>0.91544117647058798</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <v>1008287.14299</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P17">
         <v>1608.5055696074701</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P18">
         <v>1254.92984463937</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>0.81617647058823495</v>
       </c>
     </row>
-    <row r="19" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P19">
         <v>1352.9212213830299</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>0.81617647058823495</v>
       </c>
     </row>
-    <row r="20" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P20">
         <v>1472.54042762412</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="21" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P21">
         <v>1528.95166956412</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>0.81985294117647001</v>
       </c>
     </row>
-    <row r="22" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P22">
         <v>1663.9047110839299</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="23" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P23">
         <v>1551.94508748353</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>0.66176470588235303</v>
       </c>
     </row>
-    <row r="24" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P24">
         <v>2156.4207065729001</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>0.60294117647058798</v>
       </c>
     </row>
-    <row r="25" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P25">
         <v>2273.3309522936602</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>0.39705882352941102</v>
       </c>
     </row>
-    <row r="26" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P26">
         <v>2450.8443254601498</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="27" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P27">
         <v>3099.5348132387398</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="28" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P28">
         <v>5296.0195526859297</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="29" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P29">
         <v>5090.0575080803101</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>0.54411764705882304</v>
       </c>
     </row>
-    <row r="30" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P30">
         <v>5324.6432593392001</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>0.49264705882352899</v>
       </c>
     </row>
-    <row r="31" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P31">
         <v>7126.5797989979101</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0.496323529411764</v>
       </c>
     </row>
-    <row r="32" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="16:20" x14ac:dyDescent="0.25">
       <c r="P32">
         <v>8205.51119349898</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>0.496323529411764</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P33">
         <v>12154.970287534299</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>0.44852941176470501</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P34">
         <v>25018.3868587463</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>0.40073529411764702</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>45</v>
       </c>
@@ -3659,7 +3659,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
     </row>
-    <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P52" s="15" t="s">
         <v>61</v>
       </c>
@@ -3694,7 +3694,7 @@
       <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3708,13 +3708,13 @@
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="12.54296875" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="26" width="12.5703125" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="E1" s="15"/>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>296.10389610389598</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>454.68159000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>322.72727272727201</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>467.34913999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>348.05194805194799</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>488.52064999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>373.376623376623</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>509.65287000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>398.05194805194799</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>522.20258000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>423.376623376623</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>543.35445000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>447.402597402597</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>551.60307999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>472.72727272727201</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>572.75495000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>498.05194805194799</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>585.30466000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>522.72727272727195</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>610.73796000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>548.05194805194799</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>653.39520000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>572.72727272727195</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>721.85888999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>598.05194805194799</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>803.22581000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>622.72727272727195</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>901.79701999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>648.05194805194799</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>1026.1550500000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>673.376623376623</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>583.95378690629002</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>698.05194805194799</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>597.04749679075701</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>722.72727272727195</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>611.68164313221996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>747.40259740259705</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>628.62644415917805</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>773.376623376623</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>655.58408215661098</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>797.40259740259705</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>687.16302952503202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>822.72727272727195</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>721.05263157894694</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>847.40259740259705</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>764.18485237483901</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>872.72727272727195</v>
       </c>
@@ -4020,10 +4020,10 @@
         <v>801.155327342747</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="Y36" s="7"/>
     </row>
-    <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>8</v>
       </c>
@@ -4033,7 +4033,7 @@
       </c>
       <c r="E47" s="15"/>
     </row>
-    <row r="49" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>5</v>
       </c>
@@ -4061,13 +4061,13 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="12.54296875" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="26" width="12.5703125" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="E1" s="15"/>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>295.83333333333297</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>28.158940000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>322.61904761904702</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>28.887419999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>372.61904761904702</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>29.748339999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>473.21428571428498</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>30.27815</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>572.61904761904702</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>30.344370000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>672.61904761904702</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>30.211919999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>772.61904761904702</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>29.947019999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>872.61904761904702</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>29.682120000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <v>401.36986000000002</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>29.483440000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <v>450.68493000000001</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>29.350989999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <v>502.73973000000001</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>29.61589</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <v>552.05479000000003</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>30.079470000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <v>601.36986000000002</v>
       </c>
@@ -4243,10 +4243,10 @@
         <v>31.13907</v>
       </c>
     </row>
-    <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>9</v>
       </c>
@@ -4256,12 +4256,12 @@
       </c>
       <c r="E33" s="15"/>
     </row>
-    <row r="35" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="V39" s="7"/>
     </row>
   </sheetData>
@@ -4287,17 +4287,17 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" style="10"/>
-    <col min="4" max="4" width="16.453125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="10"/>
+    <col min="1" max="1" width="15.42578125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="10"/>
+    <col min="4" max="4" width="16.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -4305,13 +4305,13 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4321,7 +4321,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>303.31797235022998</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>51.077844311377198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>327.64976958525301</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>54.550898203592801</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>344.23963133640501</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>56.467065868263397</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>365.806451612903</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>59.101796407185603</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>396.22119815668202</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>62.814371257485</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>423.31797235022998</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>66.407185628742496</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>450.41474654377799</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>69.281437125748496</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>467.00460829492999</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>71.437125748502893</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>497.41935483870901</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>75.508982035928099</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>523.41013824884703</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>77.425149700598794</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>545.52995391704997</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>81.137724550898199</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>577.05069124423903</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>84.730538922155603</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>601.935483870967</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>87.245508982035901</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>657.78801843317899</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>93.473053892215503</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>682.11981566820202</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>96.227544910179603</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>708.11059907834101</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>99.580838323353206</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>734.65437788018403</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>102.57485029940101</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>763.41013824884703</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>105.808383233532</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>783.87096774193503</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>107.96407185628701</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>817.05069124423903</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>111.19760479041901</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>850.23041474654303</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>114.19161676646701</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>883.963133640553</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>117.425149700598</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>924.88479262672797</v>
       </c>
@@ -4505,16 +4505,16 @@
         <v>121.377245508982</v>
       </c>
     </row>
-    <row r="37" spans="22:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="22:22" x14ac:dyDescent="0.25">
       <c r="V37" s="12"/>
     </row>
-    <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B53" s="15"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>5</v>
       </c>
@@ -4541,18 +4541,18 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="15"/>
     </row>
-    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>100</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>10.6898734177215</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>200</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>11.0443037974683</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>300</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>11.386075949366999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>400</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>11.6962025316455</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>500</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>11.987341772151799</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>600</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>12.246835443037901</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>700</v>
       </c>
@@ -4616,13 +4616,13 @@
         <v>12.487341772151799</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B39" s="15"/>
     </row>
-    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
@@ -4648,12 +4648,12 @@
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
@@ -4668,7 +4668,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>473.100871731008</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>8.3535353535353393E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>573.22540473225399</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>0.10090909090909</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>672.97633872976303</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>0.12030303030303</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>772.72727272727195</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>0.14070707070707</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>872.851805728518</v>
       </c>
@@ -4806,11 +4806,11 @@
         <v>0.16292929292929201</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -4825,7 +4825,7 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>24</v>
       </c>
@@ -4847,7 +4847,7 @@
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
     </row>
-    <row r="34" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>20</v>
       </c>
@@ -4877,19 +4877,19 @@
       <selection activeCell="A27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="5" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="5"/>
+    <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>17.541148288385699</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>33.767998351492601</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>147.82474306467799</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>32.228318264945997</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>297.73587821652097</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>36.684439636298002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>447.708832393168</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>40.214563531926899</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>498.24588517116098</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>33.211627128248601</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>548.53566184993394</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>29.912680627463001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>599.16544316513398</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>21.520748010200101</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>648.18792983540595</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>20.538083095072398</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>698.81771115060599</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>12.1461504778094</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="179.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>69</v>
       </c>
@@ -4989,16 +4989,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689ABF1C-EFBF-442E-A0BE-50F31494446C}">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="T1" s="15"/>
     </row>
-    <row r="3" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>20</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>50</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>100</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>150</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>200</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>250</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>300</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>495.42626000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>350</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>466.57317999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>400</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>432.49275</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>450</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>389.26197000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>500</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>339.49808999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>550</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>276.65652999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>600</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>199.44013000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>650</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>105.22734</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>700</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>137.14859437750999</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>17</v>
       </c>
@@ -5481,7 +5481,7 @@
       <c r="S39" s="15"/>
       <c r="T39" s="15"/>
     </row>
-    <row r="40" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
@@ -5511,16 +5511,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96129535-FEF3-45F0-8A22-F7741A343589}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.54296875" style="1"/>
+    <col min="1" max="16384" width="12.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
@@ -5545,7 +5545,7 @@
       <c r="R1" s="14"/>
       <c r="S1" s="14"/>
     </row>
-    <row r="3" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>7.3191884470258204</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>50</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>9.1572334498903505</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100</v>
       </c>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>150</v>
       </c>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>200</v>
       </c>
@@ -5820,7 +5820,7 @@
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>250</v>
       </c>
@@ -5858,7 +5858,7 @@
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>300</v>
       </c>
@@ -5889,7 +5889,7 @@
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>350</v>
       </c>
@@ -5908,7 +5908,7 @@
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>400</v>
       </c>
@@ -5923,7 +5923,7 @@
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>450</v>
       </c>
@@ -5938,7 +5938,7 @@
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>500</v>
       </c>
@@ -5953,7 +5953,7 @@
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>550</v>
       </c>
@@ -5968,7 +5968,7 @@
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>600</v>
       </c>
@@ -5978,7 +5978,7 @@
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>650</v>
       </c>
@@ -5988,7 +5988,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>700</v>
       </c>
@@ -5998,7 +5998,7 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="41" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>19</v>
       </c>
@@ -6023,7 +6023,7 @@
       <c r="S41" s="14"/>
       <c r="T41" s="14"/>
     </row>
-    <row r="42" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>14</v>
       </c>

</xml_diff>